<commit_message>
Finish populate_db command Add all nine planets and sun data (except description) in db_data.xlsx
</commit_message>
<xml_diff>
--- a/src/db_data.xlsx
+++ b/src/db_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t xml:space="preserve">BODIES
 </t>
@@ -33,10 +33,7 @@
 </t>
   </si>
   <si>
-    <t>1.989 × 10^30</t>
-  </si>
-  <si>
-    <t>4.603</t>
+    <t>1.989 * 10**30</t>
   </si>
   <si>
     <t>S</t>
@@ -46,10 +43,7 @@
 </t>
   </si>
   <si>
-    <t>3.3011×10^23</t>
-  </si>
-  <si>
-    <t>4.503</t>
+    <t>3.3011*10**23</t>
   </si>
   <si>
     <t>TS</t>
@@ -59,16 +53,13 @@
 </t>
   </si>
   <si>
-    <t>4.869×10^24</t>
+    <t>4.869*10**24</t>
   </si>
   <si>
     <t>Earth</t>
   </si>
   <si>
-    <t>5.972 × 10^24</t>
-  </si>
-  <si>
-    <t>4.543</t>
+    <t>5.972 * 10**24</t>
   </si>
   <si>
     <t xml:space="preserve">TS
@@ -78,20 +69,14 @@
     <t>Mars</t>
   </si>
   <si>
-    <t>6.39 × 10^23</t>
-  </si>
-  <si>
-    <t>3 389.5</t>
+    <t>6.39 * 10**23</t>
   </si>
   <si>
     <t xml:space="preserve">Jupiter
 </t>
   </si>
   <si>
-    <t>1.898 × 10^27</t>
-  </si>
-  <si>
-    <t>69 911</t>
+    <t>1.898 * 10**27</t>
   </si>
   <si>
     <t>GG</t>
@@ -100,10 +85,7 @@
     <t>Saturn</t>
   </si>
   <si>
-    <t>5.683 × 10^26</t>
-  </si>
-  <si>
-    <t>58 232</t>
+    <t>5.683 * 10**26</t>
   </si>
   <si>
     <t xml:space="preserve">GG
@@ -113,10 +95,7 @@
     <t>Uranus</t>
   </si>
   <si>
-    <t>8.681 × 10^25</t>
-  </si>
-  <si>
-    <t>25 362</t>
+    <t>8.681 * 10**25</t>
   </si>
   <si>
     <t>IC</t>
@@ -126,33 +105,27 @@
 </t>
   </si>
   <si>
-    <t>1.024 × 10^26</t>
-  </si>
-  <si>
-    <t>24 622</t>
+    <t>1.024 * 10**26</t>
   </si>
   <si>
     <t>Pluto</t>
   </si>
   <si>
-    <t>1.30900 × 10^22</t>
-  </si>
-  <si>
-    <t>1 188.3</t>
+    <t>1.30900 * 10**22</t>
   </si>
   <si>
     <t>DP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy.m"/>
-    <numFmt numFmtId="165" formatCode="d.m"/>
-  </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -162,6 +135,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -188,16 +162,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -451,170 +425,175 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>695510.0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3">
+        <v>4.603</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2">
+        <v>2439.7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4.503</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="3">
-        <v>197049.0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1516336.0</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6051.8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4.503</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="2">
         <v>6371.0</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
+      <c r="D5" s="3">
+        <v>4.543</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3389.5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4.603</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3">
+        <v>69911.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4.503</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3">
+        <v>58232.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4.503</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25362.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4.503</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3">
+        <v>24622.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4.503</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="5">
-        <v>43589.0</v>
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1188.3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4.5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cb_descriptions command to django (it extracts descriptions from cb_descriptions.txt) Remove newline character from excel cells
</commit_message>
<xml_diff>
--- a/src/db_data.xlsx
+++ b/src/db_data.xlsx
@@ -29,8 +29,7 @@
     <t>BODY_TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">Sun
-</t>
+    <t>Sun</t>
   </si>
   <si>
     <t>1.989 * 10**30</t>
@@ -39,8 +38,7 @@
     <t>S</t>
   </si>
   <si>
-    <t xml:space="preserve">Mercury
-</t>
+    <t>Mercury</t>
   </si>
   <si>
     <t>3.3011*10**23</t>
@@ -49,8 +47,7 @@
     <t>TS</t>
   </si>
   <si>
-    <t xml:space="preserve">Venus
-</t>
+    <t>Venus</t>
   </si>
   <si>
     <t>4.869*10**24</t>
@@ -72,8 +69,7 @@
     <t>6.39 * 10**23</t>
   </si>
   <si>
-    <t xml:space="preserve">Jupiter
-</t>
+    <t>Jupiter</t>
   </si>
   <si>
     <t>1.898 * 10**27</t>
@@ -101,8 +97,7 @@
     <t>IC</t>
   </si>
   <si>
-    <t xml:space="preserve">Neptune
-</t>
+    <t>Neptune</t>
   </si>
   <si>
     <t>1.024 * 10**26</t>
@@ -125,7 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -135,7 +130,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -162,13 +156,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -422,16 +416,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>695510.0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>4.603</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -439,16 +433,16 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>2439.7</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>4.503</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -456,16 +450,16 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>6051.8</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>4.503</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -473,16 +467,16 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>6371.0</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>4.543</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -490,16 +484,16 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>3389.5</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>4.603</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -507,16 +501,16 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>69911.0</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>4.503</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -524,16 +518,16 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>58232.0</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>4.503</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -541,16 +535,16 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>25362.0</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>4.503</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -558,16 +552,16 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>24622.0</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>4.503</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -575,16 +569,16 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="1">
         <v>1188.3</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="4">
         <v>4.5</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -592,7 +586,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>